<commit_message>
POP read excel data
</commit_message>
<xml_diff>
--- a/src/test/resources/frazy.xlsx
+++ b/src/test/resources/frazy.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,23 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zbigniew.gornowicz\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD9E04BE-C360-402B-A43E-A08EDD9403D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD419245-EB4E-4342-BAA3-4860A581D1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -40,14 +31,14 @@
     <t>Brudny Harry</t>
   </si>
   <si>
-    <t>Słowo</t>
+    <t>Fraza</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +53,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -79,7 +76,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -102,14 +99,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -384,11 +394,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,26 +407,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>